<commit_message>
Finished program parse and started working on schedule generation
</commit_message>
<xml_diff>
--- a/Schedulator/Programs.xlsx
+++ b/Schedulator/Programs.xlsx
@@ -14,6 +14,10 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+    <definedName name="LOCAL_SECOND_FORMAT" hidden="1">" "</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -29,9 +33,6 @@
     <t>Year 1</t>
   </si>
   <si>
-    <t>Year 1 – Fall</t>
-  </si>
-  <si>
     <t>Course Number</t>
   </si>
   <si>
@@ -68,9 +69,6 @@
     <t>General Elective</t>
   </si>
   <si>
-    <t>Year 1 – Winter</t>
-  </si>
-  <si>
     <t>COMP 249</t>
   </si>
   <si>
@@ -101,9 +99,6 @@
     <t>Year 2</t>
   </si>
   <si>
-    <t>Year 2 – Fall</t>
-  </si>
-  <si>
     <t>COMP 348</t>
   </si>
   <si>
@@ -128,9 +123,6 @@
     <t>Sustainable Development and Environmental Stewardship</t>
   </si>
   <si>
-    <t>Year 2 – Winter</t>
-  </si>
-  <si>
     <t>COMP 346</t>
   </si>
   <si>
@@ -164,9 +156,6 @@
     <t>Year 3</t>
   </si>
   <si>
-    <t>Year 3 – Fall</t>
-  </si>
-  <si>
     <t>COMP 335</t>
   </si>
   <si>
@@ -197,9 +186,6 @@
     <t>Numerical Methods in Engineering</t>
   </si>
   <si>
-    <t>Year 3 – Winter</t>
-  </si>
-  <si>
     <t>SOEN 344</t>
   </si>
   <si>
@@ -233,9 +219,6 @@
     <t>Year 4</t>
   </si>
   <si>
-    <t>Year 4 – Fall</t>
-  </si>
-  <si>
     <t>SOEN 490</t>
   </si>
   <si>
@@ -287,9 +270,6 @@
     <t>Artificial Intelligence</t>
   </si>
   <si>
-    <t>Year 4 – Winter</t>
-  </si>
-  <si>
     <t>SOEN 385</t>
   </si>
   <si>
@@ -302,16 +282,40 @@
     <t>Impact of Technology on Society</t>
   </si>
   <si>
+    <t>Advanced Game Development</t>
+  </si>
+  <si>
+    <t>Software Engineering</t>
+  </si>
+  <si>
+    <t>Computer Games</t>
+  </si>
+  <si>
+    <t>Year 1 Fall</t>
+  </si>
+  <si>
+    <t>Year 1 Winter</t>
+  </si>
+  <si>
+    <t>Year 2 Fall</t>
+  </si>
+  <si>
+    <t>Year 2 Winter</t>
+  </si>
+  <si>
+    <t>Year 3 Fall</t>
+  </si>
+  <si>
+    <t>Year 3 Winter</t>
+  </si>
+  <si>
+    <t>Year 4 Fall</t>
+  </si>
+  <si>
+    <t>Year 4 Winter</t>
+  </si>
+  <si>
     <t>COMP 476 or</t>
-  </si>
-  <si>
-    <t>Advanced Game Development</t>
-  </si>
-  <si>
-    <t>Software Engineering</t>
-  </si>
-  <si>
-    <t>Computer Games</t>
   </si>
 </sst>
 </file>
@@ -414,7 +418,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -428,12 +432,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -443,14 +441,17 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -461,21 +462,40 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -752,8 +772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A69" sqref="A69"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="A70" sqref="A70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -766,10 +786,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="B1" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="C1">
         <v>120</v>
@@ -781,29 +801,29 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
+      <c r="A3" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
     </row>
     <row r="4" spans="1:3" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>3</v>
-      </c>
       <c r="C4" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="48.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>6</v>
       </c>
       <c r="C5" s="3">
         <v>3</v>
@@ -811,10 +831,10 @@
     </row>
     <row r="6" spans="1:3" ht="48.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>8</v>
       </c>
       <c r="C6" s="4">
         <v>3</v>
@@ -822,10 +842,10 @@
     </row>
     <row r="7" spans="1:3" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>10</v>
       </c>
       <c r="C7" s="3">
         <v>1.5</v>
@@ -833,10 +853,10 @@
     </row>
     <row r="8" spans="1:3" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>12</v>
       </c>
       <c r="C8" s="4">
         <v>3</v>
@@ -844,40 +864,40 @@
     </row>
     <row r="9" spans="1:3" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
     </row>
     <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
     </row>
     <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
+      <c r="A11" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
     </row>
     <row r="12" spans="1:3" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>3</v>
-      </c>
       <c r="C12" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="48.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C13" s="3">
         <v>3</v>
@@ -885,10 +905,10 @@
     </row>
     <row r="14" spans="1:3" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C14" s="4">
         <v>3</v>
@@ -896,10 +916,10 @@
     </row>
     <row r="15" spans="1:3" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C15" s="3">
         <v>4</v>
@@ -907,10 +927,10 @@
     </row>
     <row r="16" spans="1:3" ht="48.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C16" s="4">
         <v>3</v>
@@ -918,147 +938,147 @@
     </row>
     <row r="17" spans="1:3" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
     </row>
     <row r="18" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
+      <c r="A19" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
     </row>
     <row r="20" spans="1:3" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>3</v>
-      </c>
       <c r="C20" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="72.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="C22" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
+      <c r="B23" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="C23" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
+      <c r="B24" s="4" t="s">
         <v>30</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C23" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="96.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>33</v>
       </c>
       <c r="C24" s="4">
         <v>1.5</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
     </row>
     <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="6"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
+      <c r="A26" s="10"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
     </row>
     <row r="27" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-    </row>
-    <row r="28" spans="1:3" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+    </row>
+    <row r="28" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C28" s="4">
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C29" s="3">
         <v>3.5</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="72.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C30" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B32" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="C30" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="96.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C31" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>44</v>
       </c>
       <c r="C32" s="4">
         <v>3</v>
@@ -1066,155 +1086,155 @@
     </row>
     <row r="33" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="B34" s="11"/>
+      <c r="C34" s="11"/>
+    </row>
+    <row r="35" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C36" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B37" s="4" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="5" t="s">
+      <c r="C37" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
-    </row>
-    <row r="35" spans="1:3" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
+      <c r="B38" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C38" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C39" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C40" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="10"/>
+      <c r="B41" s="10"/>
+      <c r="C41" s="10"/>
+    </row>
+    <row r="42" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="B42" s="11"/>
+      <c r="C42" s="11"/>
+    </row>
+    <row r="43" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="72.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C36" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C37" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="48.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B38" s="3" t="s">
+      <c r="C43" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C38" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="72.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="4" t="s">
+      <c r="B44" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="C44" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C39" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="3" t="s">
+      <c r="B45" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="C45" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C40" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="6"/>
-      <c r="B41" s="6"/>
-      <c r="C41" s="6"/>
-    </row>
-    <row r="42" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="5" t="s">
+      <c r="B46" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B42" s="5"/>
-      <c r="C42" s="5"/>
-    </row>
-    <row r="43" spans="1:3" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="48.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="3" t="s">
+      <c r="C46" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B47" s="4" t="s">
         <v>59</v>
-      </c>
-      <c r="C44" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="84.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C45" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C46" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>65</v>
       </c>
       <c r="C47" s="4">
         <v>3.5</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C48" s="3">
         <v>4</v>
@@ -1222,230 +1242,230 @@
     </row>
     <row r="49" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="B50" s="5"/>
-      <c r="C50" s="5"/>
-    </row>
-    <row r="51" spans="1:3" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="B50" s="11"/>
+      <c r="C50" s="11"/>
+    </row>
+    <row r="51" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B51" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B51" s="2" t="s">
-        <v>3</v>
-      </c>
       <c r="C51" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C52" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="96.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C53" s="4">
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="48.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C54" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="48.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C55" s="4">
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="24" x14ac:dyDescent="0.25">
-      <c r="A56" s="8" t="s">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B56" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C56" s="12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B57" s="13"/>
+      <c r="C57" s="13"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B58" s="13"/>
+      <c r="C58" s="13"/>
+    </row>
+    <row r="59" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B59" s="14"/>
+      <c r="C59" s="14"/>
+    </row>
+    <row r="60" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C60" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B56" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="C56" s="13">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="24" x14ac:dyDescent="0.25">
-      <c r="A57" s="7" t="s">
+      <c r="B61" s="3" t="s">
         <v>79</v>
-      </c>
-      <c r="B57" s="14"/>
-      <c r="C57" s="14"/>
-    </row>
-    <row r="58" spans="1:3" ht="24" x14ac:dyDescent="0.25">
-      <c r="A58" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="B58" s="14"/>
-      <c r="C58" s="14"/>
-    </row>
-    <row r="59" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="B59" s="15"/>
-      <c r="C59" s="15"/>
-    </row>
-    <row r="60" spans="1:3" ht="48.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="B60" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C60" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" ht="48.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>86</v>
       </c>
       <c r="C61" s="3">
         <v>4</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="6"/>
-      <c r="B62" s="6"/>
-      <c r="C62" s="6"/>
+      <c r="A62" s="10"/>
+      <c r="B62" s="10"/>
+      <c r="C62" s="10"/>
     </row>
     <row r="63" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="B63" s="5"/>
-      <c r="C63" s="5"/>
-    </row>
-    <row r="64" spans="1:3" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="B63" s="11"/>
+      <c r="C63" s="11"/>
+    </row>
+    <row r="64" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B64" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B64" s="2" t="s">
-        <v>3</v>
-      </c>
       <c r="C64" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="C65" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="48.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="4" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C66" s="4">
         <v>3</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C67" s="3">
         <v>-4</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="24" x14ac:dyDescent="0.25">
-      <c r="A68" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="B68" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="C68" s="16">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B68" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="C68" s="12">
         <v>4</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="10" t="s">
+      <c r="A69" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B69" s="13"/>
+      <c r="C69" s="13"/>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B70" s="13"/>
+      <c r="C70" s="13"/>
+    </row>
+    <row r="71" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B71" s="14"/>
+      <c r="C71" s="14"/>
+    </row>
+    <row r="72" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C72" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B73" s="4" t="s">
         <v>79</v>
-      </c>
-      <c r="B69" s="17"/>
-      <c r="C69" s="17"/>
-    </row>
-    <row r="70" spans="1:3" ht="24" x14ac:dyDescent="0.25">
-      <c r="A70" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="B70" s="17"/>
-      <c r="C70" s="17"/>
-    </row>
-    <row r="71" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="B71" s="18"/>
-      <c r="C71" s="18"/>
-    </row>
-    <row r="72" spans="1:3" ht="48.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C72" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" ht="48.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="B73" s="4" t="s">
-        <v>86</v>
       </c>
       <c r="C73" s="4">
         <v>4</v>
@@ -1453,22 +1473,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B68:B71"/>
+    <mergeCell ref="C68:C71"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A26:C26"/>
     <mergeCell ref="A62:C62"/>
     <mergeCell ref="A63:C63"/>
-    <mergeCell ref="B68:B71"/>
-    <mergeCell ref="C68:C71"/>
     <mergeCell ref="A34:C34"/>
     <mergeCell ref="A41:C41"/>
     <mergeCell ref="A42:C42"/>
     <mergeCell ref="A50:C50"/>
     <mergeCell ref="B56:B59"/>
     <mergeCell ref="C56:C59"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="A27:C27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Added program management to program director
</commit_message>
<xml_diff>
--- a/Schedulator/Programs.xlsx
+++ b/Schedulator/Programs.xlsx
@@ -12,7 +12,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="12570"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="SOEN COMP GAMES SEPT" sheetId="1" r:id="rId1"/>
+    <sheet name="SOEN COMP GAMES JAN" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="97">
   <si>
     <t>Year 1</t>
   </si>
@@ -316,6 +317,9 @@
   </si>
   <si>
     <t>COMP 476 or</t>
+  </si>
+  <si>
+    <t>Septemeber</t>
   </si>
 </sst>
 </file>
@@ -447,12 +451,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -461,6 +459,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -770,10 +774,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C73"/>
+  <dimension ref="A1:D73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="A70" sqref="A70"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -784,30 +788,33 @@
     <col min="4" max="4" width="38.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>85</v>
       </c>
       <c r="B1" t="s">
         <v>86</v>
       </c>
-      <c r="C1">
+      <c r="C1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1">
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="11" t="s">
+    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-    </row>
-    <row r="4" spans="1:3" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+    </row>
+    <row r="4" spans="1:4" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -818,7 +825,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="48.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="48.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -829,7 +836,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="48.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="48.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
@@ -840,7 +847,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
@@ -851,7 +858,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>10</v>
       </c>
@@ -862,26 +869,26 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
     </row>
-    <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-    </row>
-    <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="11" t="s">
+    <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="14"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+    </row>
+    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-    </row>
-    <row r="12" spans="1:3" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+    </row>
+    <row r="12" spans="1:4" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
@@ -892,7 +899,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="48.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="48.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
@@ -903,7 +910,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>15</v>
       </c>
@@ -914,7 +921,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>17</v>
       </c>
@@ -925,7 +932,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="48.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="48.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>19</v>
       </c>
@@ -949,11 +956,11 @@
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
     </row>
     <row r="20" spans="1:3" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
@@ -1018,16 +1025,16 @@
       <c r="C25" s="3"/>
     </row>
     <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="10"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="10"/>
+      <c r="A26" s="14"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
     </row>
     <row r="27" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="11" t="s">
+      <c r="A27" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="B27" s="11"/>
-      <c r="C27" s="11"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="13"/>
     </row>
     <row r="28" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
@@ -1090,11 +1097,11 @@
       </c>
     </row>
     <row r="34" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="11" t="s">
+      <c r="A34" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="B34" s="11"/>
-      <c r="C34" s="11"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="13"/>
     </row>
     <row r="35" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
@@ -1163,16 +1170,16 @@
       </c>
     </row>
     <row r="41" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="10"/>
-      <c r="B41" s="10"/>
-      <c r="C41" s="10"/>
+      <c r="A41" s="14"/>
+      <c r="B41" s="14"/>
+      <c r="C41" s="14"/>
     </row>
     <row r="42" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="11" t="s">
+      <c r="A42" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="B42" s="11"/>
-      <c r="C42" s="11"/>
+      <c r="B42" s="13"/>
+      <c r="C42" s="13"/>
     </row>
     <row r="43" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
@@ -1246,11 +1253,11 @@
       </c>
     </row>
     <row r="50" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="11" t="s">
+      <c r="A50" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="B50" s="11"/>
-      <c r="C50" s="11"/>
+      <c r="B50" s="13"/>
+      <c r="C50" s="13"/>
     </row>
     <row r="51" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
@@ -1311,10 +1318,10 @@
       <c r="A56" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="B56" s="12" t="s">
+      <c r="B56" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="C56" s="12">
+      <c r="C56" s="10">
         <v>4</v>
       </c>
     </row>
@@ -1322,22 +1329,22 @@
       <c r="A57" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B57" s="13"/>
-      <c r="C57" s="13"/>
+      <c r="B57" s="11"/>
+      <c r="C57" s="11"/>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B58" s="13"/>
-      <c r="C58" s="13"/>
+      <c r="B58" s="11"/>
+      <c r="C58" s="11"/>
     </row>
     <row r="59" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="B59" s="14"/>
-      <c r="C59" s="14"/>
+      <c r="B59" s="12"/>
+      <c r="C59" s="12"/>
     </row>
     <row r="60" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="4" t="s">
@@ -1362,16 +1369,16 @@
       </c>
     </row>
     <row r="62" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="10"/>
-      <c r="B62" s="10"/>
-      <c r="C62" s="10"/>
+      <c r="A62" s="14"/>
+      <c r="B62" s="14"/>
+      <c r="C62" s="14"/>
     </row>
     <row r="63" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="11" t="s">
+      <c r="A63" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="B63" s="11"/>
-      <c r="C63" s="11"/>
+      <c r="B63" s="13"/>
+      <c r="C63" s="13"/>
     </row>
     <row r="64" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
@@ -1421,10 +1428,10 @@
       <c r="A68" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="B68" s="12" t="s">
+      <c r="B68" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="C68" s="12">
+      <c r="C68" s="10">
         <v>4</v>
       </c>
     </row>
@@ -1432,22 +1439,22 @@
       <c r="A69" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B69" s="13"/>
-      <c r="C69" s="13"/>
+      <c r="B69" s="11"/>
+      <c r="C69" s="11"/>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B70" s="13"/>
-      <c r="C70" s="13"/>
+      <c r="B70" s="11"/>
+      <c r="C70" s="11"/>
     </row>
     <row r="71" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="B71" s="14"/>
-      <c r="C71" s="14"/>
+      <c r="B71" s="12"/>
+      <c r="C71" s="12"/>
     </row>
     <row r="72" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="s">
@@ -1493,4 +1500,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Changed from COMP 393 to ENCS 393 in Computer Games COMP SCI program
</commit_message>
<xml_diff>
--- a/Schedulator/Programs.xlsx
+++ b/Schedulator/Programs.xlsx
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2742" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2742" uniqueCount="167">
   <si>
     <t>Year 1</t>
   </si>
@@ -483,9 +483,6 @@
   </si>
   <si>
     <t>Introduction to Game Development </t>
-  </si>
-  <si>
-    <t>COMP 393</t>
   </si>
   <si>
     <t>COMP 361</t>
@@ -1167,7 +1164,7 @@
         <v>139</v>
       </c>
       <c r="B1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C1" t="s">
         <v>97</v>
@@ -1313,7 +1310,7 @@
     </row>
     <row r="17" spans="1:3" ht="15.75" thickBot="1">
       <c r="A17" s="24" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.75" thickBot="1">
@@ -1403,7 +1400,7 @@
     </row>
     <row r="29" spans="1:3" ht="15.75" thickBot="1">
       <c r="A29" s="35" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B29" s="35"/>
       <c r="C29" s="35"/>
@@ -1498,7 +1495,7 @@
         <v>121</v>
       </c>
       <c r="B39" s="25" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C39" s="25">
         <v>3</v>
@@ -1703,7 +1700,7 @@
     </row>
     <row r="17" spans="1:3" ht="15.75" thickBot="1">
       <c r="A17" s="24" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.75" thickBot="1">
@@ -1793,7 +1790,7 @@
     </row>
     <row r="29" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
       <c r="A29" s="35" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B29" s="35"/>
       <c r="C29" s="35"/>
@@ -1934,7 +1931,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="D41" sqref="D41:D46"/>
     </sheetView>
   </sheetViews>
@@ -2027,7 +2024,7 @@
     </row>
     <row r="10" spans="1:4" ht="15.75" customHeight="1" thickBot="1">
       <c r="A10" s="35" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B10" s="35"/>
       <c r="C10" s="35"/>
@@ -2152,7 +2149,7 @@
     </row>
     <row r="23" spans="1:3" ht="24.75" thickBot="1">
       <c r="A23" s="25" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B23" s="25" t="s">
         <v>143</v>
@@ -2366,8 +2363,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -2744,7 +2741,7 @@
     </row>
     <row r="41" spans="1:3" ht="60.75" thickBot="1">
       <c r="A41" s="27" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="B41" s="27" t="s">
         <v>138</v>
@@ -2960,7 +2957,7 @@
     </row>
     <row r="17" spans="1:3" ht="15.75" thickBot="1">
       <c r="A17" s="24" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.75" thickBot="1">
@@ -3046,7 +3043,7 @@
     </row>
     <row r="29" spans="1:3" ht="15.75" thickBot="1">
       <c r="A29" s="35" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B29" s="35"/>
       <c r="C29" s="35"/>
@@ -3276,7 +3273,7 @@
     </row>
     <row r="10" spans="1:4" ht="15.75" customHeight="1" thickBot="1">
       <c r="A10" s="35" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B10" s="35"/>
       <c r="C10" s="35"/>
@@ -4177,7 +4174,7 @@
     </row>
     <row r="17" spans="1:3" ht="15.75" thickBot="1">
       <c r="A17" s="24" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.75" thickBot="1">
@@ -4263,7 +4260,7 @@
     </row>
     <row r="29" spans="1:3" ht="15.75" thickBot="1">
       <c r="A29" s="35" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B29" s="35"/>
       <c r="C29" s="35"/>
@@ -4489,7 +4486,7 @@
     </row>
     <row r="10" spans="1:4" ht="15.75" customHeight="1" thickBot="1">
       <c r="A10" s="35" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B10" s="35"/>
       <c r="C10" s="35"/>
@@ -5801,7 +5798,7 @@
     </row>
     <row r="60" spans="1:3" ht="15.75" thickBot="1">
       <c r="A60" s="34" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B60" s="4" t="s">
         <v>76</v>
@@ -5900,10 +5897,10 @@
     </row>
     <row r="71" spans="1:3" ht="15.75" thickBot="1">
       <c r="A71" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="B71" s="4" t="s">
         <v>163</v>
-      </c>
-      <c r="B71" s="4" t="s">
-        <v>164</v>
       </c>
       <c r="C71" s="4">
         <v>4</v>
@@ -5953,7 +5950,7 @@
         <v>139</v>
       </c>
       <c r="B1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C1" t="s">
         <v>94</v>
@@ -6030,7 +6027,7 @@
     </row>
     <row r="10" spans="1:4" ht="15.75" thickBot="1">
       <c r="A10" s="35" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B10" s="35"/>
       <c r="C10" s="35"/>
@@ -6264,7 +6261,7 @@
         <v>121</v>
       </c>
       <c r="B35" s="25" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C35" s="25">
         <v>3</v>
@@ -6469,7 +6466,7 @@
     </row>
     <row r="11" spans="1:4" ht="15.75" thickBot="1">
       <c r="A11" s="43" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B11" s="43"/>
       <c r="C11" s="43"/>
@@ -7185,7 +7182,7 @@
     </row>
     <row r="19" spans="1:3" ht="15.75" thickBot="1">
       <c r="A19" s="43" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B19" s="43"/>
       <c r="C19" s="43"/>
@@ -7360,7 +7357,7 @@
     </row>
     <row r="38" spans="1:3" ht="15.75" thickBot="1">
       <c r="A38" s="53" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B38" s="53"/>
       <c r="C38" s="53"/>
@@ -7545,7 +7542,7 @@
     </row>
     <row r="57" spans="1:3" ht="15.75" thickBot="1">
       <c r="A57" s="43" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B57" s="43"/>
       <c r="C57" s="43"/>
@@ -7662,7 +7659,7 @@
     </row>
     <row r="70" spans="1:3" ht="15.75" thickBot="1">
       <c r="A70" s="34" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B70" s="4" t="s">
         <v>76</v>
@@ -7761,10 +7758,10 @@
     </row>
     <row r="81" spans="1:3" ht="15.75" thickBot="1">
       <c r="A81" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="B81" s="4" t="s">
         <v>163</v>
-      </c>
-      <c r="B81" s="4" t="s">
-        <v>164</v>
       </c>
       <c r="C81" s="4">
         <v>4</v>
@@ -8585,7 +8582,7 @@
     </row>
     <row r="11" spans="1:4" ht="15.75" thickBot="1">
       <c r="A11" s="43" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B11" s="43"/>
       <c r="C11" s="43"/>
@@ -9327,7 +9324,7 @@
     </row>
     <row r="19" spans="1:3" ht="15.75" thickBot="1">
       <c r="A19" s="43" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B19" s="43"/>
       <c r="C19" s="43"/>
@@ -9502,7 +9499,7 @@
     </row>
     <row r="38" spans="1:3" ht="15.75" thickBot="1">
       <c r="A38" s="53" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B38" s="53"/>
       <c r="C38" s="53"/>
@@ -9690,7 +9687,7 @@
     </row>
     <row r="58" spans="1:3" ht="15.75" thickBot="1">
       <c r="A58" s="43" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B58" s="43"/>
       <c r="C58" s="43"/>
@@ -10658,7 +10655,7 @@
     </row>
     <row r="11" spans="1:4" ht="15.75" thickBot="1">
       <c r="A11" s="43" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B11" s="43"/>
       <c r="C11" s="43"/>
@@ -11376,7 +11373,7 @@
     </row>
     <row r="19" spans="1:4" ht="15.75" thickBot="1">
       <c r="A19" s="43" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B19" s="43"/>
       <c r="C19" s="43"/>
@@ -11550,7 +11547,7 @@
     </row>
     <row r="38" spans="1:3" ht="15.75" thickBot="1">
       <c r="A38" s="54" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B38" s="54"/>
       <c r="C38" s="54"/>
@@ -11738,7 +11735,7 @@
     </row>
     <row r="58" spans="1:3" ht="15.75" thickBot="1">
       <c r="A58" s="43" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B58" s="43"/>
       <c r="C58" s="43"/>
@@ -12692,7 +12689,7 @@
     </row>
     <row r="11" spans="1:4" ht="15.75" thickBot="1">
       <c r="A11" s="43" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B11" s="43"/>
       <c r="C11" s="43"/>
@@ -13238,7 +13235,7 @@
         <v>139</v>
       </c>
       <c r="B1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C1" t="s">
         <v>93</v>
@@ -13549,7 +13546,7 @@
         <v>121</v>
       </c>
       <c r="B35" s="25" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C35" s="25">
         <v>3</v>
@@ -13824,7 +13821,7 @@
     </row>
     <row r="19" spans="1:3" ht="15.75" thickBot="1">
       <c r="A19" s="43" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B19" s="43"/>
       <c r="C19" s="43"/>
@@ -13997,7 +13994,7 @@
     </row>
     <row r="38" spans="1:3" ht="15.75" thickBot="1">
       <c r="A38" s="53" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B38" s="53"/>
       <c r="C38" s="53"/>
@@ -14181,7 +14178,7 @@
     </row>
     <row r="58" spans="1:3" ht="15.75" thickBot="1">
       <c r="A58" s="43" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B58" s="43"/>
       <c r="C58" s="43"/>
@@ -14380,7 +14377,7 @@
         <v>139</v>
       </c>
       <c r="B1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C1" t="s">
         <v>97</v>
@@ -14526,7 +14523,7 @@
     </row>
     <row r="17" spans="1:3" ht="15.75" thickBot="1">
       <c r="A17" s="24" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.75" thickBot="1">
@@ -14581,7 +14578,7 @@
     </row>
     <row r="24" spans="1:3" ht="24.75" thickBot="1">
       <c r="A24" s="27" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B24" s="27" t="s">
         <v>143</v>
@@ -14616,7 +14613,7 @@
     </row>
     <row r="29" spans="1:3" ht="15.75" thickBot="1">
       <c r="A29" s="35" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B29" s="35"/>
       <c r="C29" s="35"/>
@@ -14704,10 +14701,10 @@
     </row>
     <row r="39" spans="1:3" ht="15.75" thickBot="1">
       <c r="A39" s="27" t="s">
+        <v>146</v>
+      </c>
+      <c r="B39" s="27" t="s">
         <v>147</v>
-      </c>
-      <c r="B39" s="27" t="s">
-        <v>148</v>
       </c>
       <c r="C39" s="27">
         <v>3</v>
@@ -14726,10 +14723,10 @@
     </row>
     <row r="41" spans="1:3" ht="24.75" thickBot="1">
       <c r="A41" s="27" t="s">
+        <v>155</v>
+      </c>
+      <c r="B41" s="27" t="s">
         <v>156</v>
-      </c>
-      <c r="B41" s="27" t="s">
-        <v>157</v>
       </c>
       <c r="C41" s="27">
         <v>3</v>
@@ -14748,7 +14745,7 @@
     </row>
     <row r="43" spans="1:3" ht="15.75" thickBot="1">
       <c r="A43" s="35" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B43" s="35"/>
       <c r="C43" s="35"/>
@@ -14839,7 +14836,7 @@
         <v>139</v>
       </c>
       <c r="B1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C1" t="s">
         <v>94</v>
@@ -14916,7 +14913,7 @@
     </row>
     <row r="10" spans="1:4" ht="15.75" thickBot="1">
       <c r="A10" s="35" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B10" s="35"/>
       <c r="C10" s="35"/>
@@ -15030,7 +15027,7 @@
     </row>
     <row r="22" spans="1:3" ht="24.75" thickBot="1">
       <c r="A22" s="27" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B22" s="27" t="s">
         <v>143</v>
@@ -15154,10 +15151,10 @@
     </row>
     <row r="36" spans="1:3" ht="15.75" thickBot="1">
       <c r="A36" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="B36" s="25" t="s">
         <v>147</v>
-      </c>
-      <c r="B36" s="25" t="s">
-        <v>148</v>
       </c>
       <c r="C36" s="25">
         <v>3</v>
@@ -15165,10 +15162,10 @@
     </row>
     <row r="37" spans="1:3" ht="24.75" thickBot="1">
       <c r="A37" s="27" t="s">
+        <v>155</v>
+      </c>
+      <c r="B37" s="27" t="s">
         <v>156</v>
-      </c>
-      <c r="B37" s="27" t="s">
-        <v>157</v>
       </c>
       <c r="C37" s="27">
         <v>3</v>
@@ -15208,7 +15205,7 @@
     </row>
     <row r="42" spans="1:3" ht="36.75" thickBot="1">
       <c r="A42" s="27" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B42" s="27" t="s">
         <v>128</v>
@@ -15275,7 +15272,7 @@
         <v>139</v>
       </c>
       <c r="B1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C1" t="s">
         <v>93</v>
@@ -15466,7 +15463,7 @@
     </row>
     <row r="22" spans="1:3" ht="24.75" thickBot="1">
       <c r="A22" s="27" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B22" s="27" t="s">
         <v>143</v>
@@ -15477,10 +15474,10 @@
     </row>
     <row r="23" spans="1:3" ht="15.75" thickBot="1">
       <c r="A23" s="25" t="s">
+        <v>153</v>
+      </c>
+      <c r="B23" s="25" t="s">
         <v>154</v>
-      </c>
-      <c r="B23" s="25" t="s">
-        <v>155</v>
       </c>
       <c r="C23" s="25">
         <v>3</v>
@@ -15594,10 +15591,10 @@
     </row>
     <row r="36" spans="1:3" ht="15.75" thickBot="1">
       <c r="A36" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="B36" s="25" t="s">
         <v>147</v>
-      </c>
-      <c r="B36" s="25" t="s">
-        <v>148</v>
       </c>
       <c r="C36" s="25">
         <v>3</v>
@@ -15605,10 +15602,10 @@
     </row>
     <row r="37" spans="1:3" ht="24.75" thickBot="1">
       <c r="A37" s="27" t="s">
+        <v>155</v>
+      </c>
+      <c r="B37" s="27" t="s">
         <v>156</v>
-      </c>
-      <c r="B37" s="27" t="s">
-        <v>157</v>
       </c>
       <c r="C37" s="27">
         <v>3</v>
@@ -15659,7 +15656,7 @@
     </row>
     <row r="43" spans="1:3" ht="24.75" thickBot="1">
       <c r="A43" s="25" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B43" s="25" t="s">
         <v>128</v>
@@ -15715,7 +15712,7 @@
         <v>139</v>
       </c>
       <c r="B1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C1" t="s">
         <v>97</v>
@@ -15861,7 +15858,7 @@
     </row>
     <row r="17" spans="1:3" ht="15.75" thickBot="1">
       <c r="A17" s="24" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.75" thickBot="1">
@@ -15951,7 +15948,7 @@
     </row>
     <row r="29" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
       <c r="A29" s="35" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B29" s="35"/>
       <c r="C29" s="35"/>
@@ -16035,10 +16032,10 @@
     </row>
     <row r="39" spans="1:3" ht="15.75" thickBot="1">
       <c r="A39" s="27" t="s">
+        <v>146</v>
+      </c>
+      <c r="B39" s="27" t="s">
         <v>147</v>
-      </c>
-      <c r="B39" s="27" t="s">
-        <v>148</v>
       </c>
       <c r="C39" s="27">
         <v>3</v>
@@ -16068,10 +16065,10 @@
     </row>
     <row r="42" spans="1:3" ht="24">
       <c r="A42" s="32" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B42" s="32" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C42" s="36">
         <v>4</v>
@@ -16079,10 +16076,10 @@
     </row>
     <row r="43" spans="1:3" ht="15.75" thickBot="1">
       <c r="A43" s="33" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B43" s="33" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C43" s="37"/>
     </row>
@@ -16105,7 +16102,7 @@
     </row>
     <row r="47" spans="1:3" ht="15.75" thickBot="1">
       <c r="A47" s="35" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B47" s="35"/>
       <c r="C47" s="35"/>
@@ -16194,7 +16191,7 @@
         <v>139</v>
       </c>
       <c r="B1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C1" t="s">
         <v>94</v>
@@ -16271,7 +16268,7 @@
     </row>
     <row r="10" spans="1:4" ht="15.75" customHeight="1" thickBot="1">
       <c r="A10" s="35" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B10" s="35"/>
       <c r="C10" s="35"/>
@@ -16516,10 +16513,10 @@
     </row>
     <row r="37" spans="1:3" ht="15.75" thickBot="1">
       <c r="A37" s="27" t="s">
+        <v>146</v>
+      </c>
+      <c r="B37" s="27" t="s">
         <v>147</v>
-      </c>
-      <c r="B37" s="27" t="s">
-        <v>148</v>
       </c>
       <c r="C37" s="27">
         <v>3</v>
@@ -16622,7 +16619,7 @@
         <v>139</v>
       </c>
       <c r="B1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C1" t="s">
         <v>93</v>
@@ -16933,10 +16930,10 @@
     </row>
     <row r="36" spans="1:3" ht="15.75" thickBot="1">
       <c r="A36" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="B36" s="25" t="s">
         <v>147</v>
-      </c>
-      <c r="B36" s="25" t="s">
-        <v>148</v>
       </c>
       <c r="C36" s="25">
         <v>3</v>

</xml_diff>